<commit_message>
creation of story 71622
</commit_message>
<xml_diff>
--- a/Data Files/Excel/appLink.xlsx
+++ b/Data Files/Excel/appLink.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tpp\7102018_TPP_Iteration18\TPP_Iteration18\Data Files\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schuyler.Jones\git\KatalonAutomation\Data Files\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>appLink</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>end date</t>
+  </si>
+  <si>
+    <t>https://login-agency-qa2.fnf.com/</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +506,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -534,8 +540,9 @@
     <hyperlink ref="B4" r:id="rId4" display="mailto:joe.laverde@ctt.com"/>
     <hyperlink ref="B5" r:id="rId5" display="mailto:lgregory@fnf.com"/>
     <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="A4" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>